<commit_message>
Fixed file upload and signal error for raw material
</commit_message>
<xml_diff>
--- a/MPS.xlsx
+++ b/MPS.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{05ABBA76-1E08-478D-9FC7-0DBB1B0838F3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{25ECB5D0-485F-4551-9991-D6A761B7260D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
-  <si>
-    <t>start</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>dueDate</t>
   </si>
@@ -43,25 +40,22 @@
     <t>running</t>
   </si>
   <si>
+    <t>corsa</t>
+  </si>
+  <si>
+    <t>mbike</t>
+  </si>
+  <si>
+    <t>pastello</t>
+  </si>
+  <si>
+    <t>metallizzato</t>
+  </si>
+  <si>
+    <t>linea</t>
+  </si>
+  <si>
     <t>blu</t>
-  </si>
-  <si>
-    <t>03/20/18 12:00:00</t>
-  </si>
-  <si>
-    <t>04/24/18 18:00:00</t>
-  </si>
-  <si>
-    <t>03/19/18 12:00:00</t>
-  </si>
-  <si>
-    <t>03/23/18 18:00:00</t>
-  </si>
-  <si>
-    <t>corsa</t>
-  </si>
-  <si>
-    <t>mountain</t>
   </si>
 </sst>
 </file>
@@ -97,10 +91,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -381,23 +376,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -411,30 +407,30 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>43311.75</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
         <v>8</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
       </c>
       <c r="F2" s="1">
         <v>1</v>
@@ -443,21 +439,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="2" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>43311.75</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
         <v>9</v>
-      </c>
-      <c r="C3">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
-        <v>7</v>
       </c>
       <c r="F3" s="1">
         <v>1</v>
@@ -466,31 +462,31 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
-      <c r="F4" s="1"/>
-      <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G4" s="1"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
-      <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
-      <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
-      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>